<commit_message>
parametersEN.xlsx translated en.md links corrected
</commit_message>
<xml_diff>
--- a/docs/Manual/source/tab/parametersEN.xlsx
+++ b/docs/Manual/source/tab/parametersEN.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="23"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="TGZ-D-48-13_26" sheetId="1" state="visible" r:id="rId3"/>
@@ -45,63 +45,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="285">
-  <si>
-    <t xml:space="preserve">NAPÁJENÍ</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="292">
+  <si>
+    <t xml:space="preserve">POWER SUPPLY</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve">Ovládací napětí</t>
+    <t xml:space="preserve">Control voltage</t>
   </si>
   <si>
     <t xml:space="preserve">24 VDC ± 10 %, 400 mA*</t>
   </si>
   <si>
-    <t xml:space="preserve">Výkonové napájecí napětí</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0–48 VDC (jištění 30A)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Instalovaný příkon pro provoz S1</t>
+    <t xml:space="preserve">Power supply voltage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0–48 VDC (fuse 30A)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Installed power consumption for S1 operation</t>
   </si>
   <si>
     <t xml:space="preserve">1 kW</t>
   </si>
   <si>
-    <t xml:space="preserve">Trvalý proud na jednu osu</t>
+    <t xml:space="preserve">Constant current on one axis</t>
   </si>
   <si>
     <t xml:space="preserve">15 A</t>
   </si>
   <si>
-    <t xml:space="preserve">Trvalý celkový proud při provozu dvou os</t>
+    <t xml:space="preserve">Continuous total current when operating two axes</t>
   </si>
   <si>
     <t xml:space="preserve">2 x 15 A</t>
   </si>
   <si>
-    <t xml:space="preserve">Maximální výstupní proud (max. 5 s)</t>
+    <t xml:space="preserve">Maximum output current (max. 5s)</t>
   </si>
   <si>
     <t xml:space="preserve">2 x 30 A</t>
   </si>
   <si>
-    <t xml:space="preserve">Ztráty při jmenovité zátěži</t>
+    <t xml:space="preserve">Losses at rated load</t>
   </si>
   <si>
     <t xml:space="preserve">20 W</t>
   </si>
   <si>
-    <t xml:space="preserve">Stupeň krytí</t>
+    <t xml:space="preserve">Protection level</t>
   </si>
   <si>
     <t xml:space="preserve">IP20</t>
   </si>
   <si>
-    <t xml:space="preserve">KOMUNIKACE</t>
+    <t xml:space="preserve">COMMUNICATION</t>
   </si>
   <si>
     <t xml:space="preserve">CAN</t>
@@ -116,13 +116,13 @@
     <t xml:space="preserve">100/1000 Mb/s, 2x RJ45</t>
   </si>
   <si>
-    <t xml:space="preserve">ETHERNET UDP (servis)</t>
+    <t xml:space="preserve">ETHERNET UDP (service)</t>
   </si>
   <si>
     <t xml:space="preserve">100/1000 Mb/s, RJ45</t>
   </si>
   <si>
-    <t xml:space="preserve">Vstupy/výstupy</t>
+    <t xml:space="preserve">Inputs/outputs</t>
   </si>
   <si>
     <t xml:space="preserve">2 AI, 8 DI, 6 DO</t>
@@ -131,49 +131,49 @@
     <t xml:space="preserve">1x 22pin WEIDMÜLLER  B2CF 3.50/22/180</t>
   </si>
   <si>
-    <t xml:space="preserve">SIGNALIZACE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED displej</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chybové hlášení, 2x7 segment LED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED signalizace (osa 1 a 2 zvlášť)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1x zelená (SERVO OK)  1x červená (SERVO ERROR)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OSTATNÍ KONEKTORY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Napájení výkonové části</t>
+    <t xml:space="preserve">SIGNALING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error message, 2x7 LED segment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED signaling(axis 1 and 2 separately)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1x green (SERVO OK)1x red (SERVO ERROR)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OTHER CONNECTORS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power supply of the power section</t>
   </si>
   <si>
     <t xml:space="preserve">1 x 2pin PHOENIX PC 5/2 2-STCL1-7,62</t>
   </si>
   <si>
-    <t xml:space="preserve">Napájení řídicí části</t>
+    <t xml:space="preserve">Power supply of the control part</t>
   </si>
   <si>
     <t xml:space="preserve">1 x 5pin WEIDMÜLLER  BCZ 3.81/05/180</t>
   </si>
   <si>
-    <t xml:space="preserve">Motorový konektor</t>
+    <t xml:space="preserve">Motor connector</t>
   </si>
   <si>
     <t xml:space="preserve">2 x 6pin WEIDMÜLLER  BLZP 5.08HC/06/180</t>
   </si>
   <si>
-    <t xml:space="preserve">Zpětnovazební konektor</t>
+    <t xml:space="preserve">Feedback connector</t>
   </si>
   <si>
     <t xml:space="preserve">2x 8pin WEIDMÜLLER  B2CF 3.50/08/180</t>
   </si>
   <si>
-    <t xml:space="preserve">Externí enkodér</t>
+    <t xml:space="preserve">External encoder</t>
   </si>
   <si>
     <t xml:space="preserve">1x 12pin WEIDMÜLLER  B2CF 3.50/12/180</t>
@@ -203,7 +203,7 @@
     <t xml:space="preserve">1 x 4pin WAGO push-in</t>
   </si>
   <si>
-    <t xml:space="preserve">Brzdový konektor</t>
+    <t xml:space="preserve">Static brake connector</t>
   </si>
   <si>
     <t xml:space="preserve">1 × 6pin WEIDMÜLLER  BLF 5.00HC/06/180F</t>
@@ -221,16 +221,16 @@
     <t xml:space="preserve">30 W</t>
   </si>
   <si>
-    <t xml:space="preserve">LED signalizace</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 x Erni šroubovací svorky M5 PRESSFIT</t>
+    <t xml:space="preserve">LED signaling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 x Erni screw M5 PRESSFIT</t>
   </si>
   <si>
     <t xml:space="preserve">1 x 5pin MOLEX micro-lock, 505570-0501</t>
   </si>
   <si>
-    <t xml:space="preserve">3 x Erni šroubovací svorky M5 PRESSFIT </t>
+    <t xml:space="preserve">3 x Erni screw M5 PRESSFIT </t>
   </si>
   <si>
     <t xml:space="preserve">1 x 4pin MOLEX micro-lock, 505570-0501</t>
@@ -281,7 +281,7 @@
     <t xml:space="preserve">2 x Pressfit M5</t>
   </si>
   <si>
-    <t xml:space="preserve">Řízení, STO, BR</t>
+    <t xml:space="preserve">Control, STO, BR</t>
   </si>
   <si>
     <t xml:space="preserve">1 x 5pin MOLEX micro-lock, 5055700501</t>
@@ -290,7 +290,7 @@
     <t xml:space="preserve">3 x Pressfit M5</t>
   </si>
   <si>
-    <t xml:space="preserve">Externí teplota, Brzda</t>
+    <t xml:space="preserve">External temp, Brake</t>
   </si>
   <si>
     <t xml:space="preserve">1 x 4pin MOLEX Micro-lock 50557005011</t>
@@ -311,13 +311,13 @@
     <t xml:space="preserve">70 W</t>
   </si>
   <si>
-    <t xml:space="preserve">DC BUS (+DC, -DC) – na PCB označeno „VCC, GND“</t>
+    <t xml:space="preserve">DC BUS (+DC, -DC) –on PCB marked as „VCC, GND“</t>
   </si>
   <si>
     <t xml:space="preserve">8 x Pressfit M8</t>
   </si>
   <si>
-    <t xml:space="preserve">Řízení, STO</t>
+    <t xml:space="preserve">Control, STO</t>
   </si>
   <si>
     <t xml:space="preserve">1 x 5pin MOLEX Micro-Lock, 5055700501</t>
@@ -341,13 +341,16 @@
     <t xml:space="preserve">300 A</t>
   </si>
   <si>
+    <t xml:space="preserve">External thermistor</t>
+  </si>
+  <si>
     <t xml:space="preserve">24 VDC ± 10 %, 500 mA*</t>
   </si>
   <si>
     <t xml:space="preserve">1 x 22pin WEIDMÜLLER  B2CF 3.50/22/180</t>
   </si>
   <si>
-    <t xml:space="preserve">1 x zelená (SERVO OK)  1x červená (SERVO ERROR)</t>
+    <t xml:space="preserve">1x green (SERVO OK) 1x red (SERVO ERROR)</t>
   </si>
   <si>
     <t xml:space="preserve">8 x Pressfit M5</t>
@@ -395,10 +398,10 @@
     <t xml:space="preserve">EMI FILTR</t>
   </si>
   <si>
-    <t xml:space="preserve">Doporučený filtr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NLMO62P72-04 nebo NLA062P72-04  </t>
+    <t xml:space="preserve">Recommended type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLMO62P72-04 or NLA062P72-04  </t>
   </si>
   <si>
     <t xml:space="preserve">24 VDC ± 10 %, 600 mA*</t>
@@ -449,6 +452,9 @@
     <t xml:space="preserve">1 x 6pin WEIDMÜLLER  BLF 7.62HP/06/180F</t>
   </si>
   <si>
+    <t xml:space="preserve">EMI FILTER</t>
+  </si>
+  <si>
     <t xml:space="preserve">NCZXX3P49-04</t>
   </si>
   <si>
@@ -461,6 +467,9 @@
     <t xml:space="preserve">7 A</t>
   </si>
   <si>
+    <t xml:space="preserve">Switching frequency</t>
+  </si>
+  <si>
     <t xml:space="preserve">400 VAC/50Hz 16A</t>
   </si>
   <si>
@@ -506,10 +515,7 @@
     <t xml:space="preserve">900 W</t>
   </si>
   <si>
-    <t xml:space="preserve">VSTUPY/VÝSTUPY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">šroubovací svorky M8x12</t>
+    <t xml:space="preserve">screw M8x12</t>
   </si>
   <si>
     <t xml:space="preserve">1 x 5pin WEIDMÜLLER  BCZ 3.81/05/180F</t>
@@ -524,97 +530,97 @@
     <t xml:space="preserve">1 x 12pin WEIDMÜLLER B2CF 3.50/12/180</t>
   </si>
   <si>
-    <t xml:space="preserve">Filtr obsahující napájecí modul TGS-560</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vstupní napětí (VAC - 50/60 Hz) </t>
+    <t xml:space="preserve">Filter already inside of TGS-560</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input voltage (VAC - 50/60 Hz) </t>
   </si>
   <si>
     <t xml:space="preserve">1 x 230 VAC </t>
   </si>
   <si>
-    <t xml:space="preserve">Maximální vstupní proud (AC) </t>
+    <t xml:space="preserve">Maximum input current (AC) </t>
   </si>
   <si>
     <t xml:space="preserve">16 A</t>
   </si>
   <si>
-    <t xml:space="preserve">Výstupní napětí (DC) </t>
+    <t xml:space="preserve">Output voltage (DC) </t>
   </si>
   <si>
     <t xml:space="preserve">320 VDC </t>
   </si>
   <si>
-    <t xml:space="preserve">Maximální trvalý výstupní proud (DC) </t>
+    <t xml:space="preserve">Maximum continuous output current (DC) </t>
   </si>
   <si>
     <t xml:space="preserve">10 A </t>
   </si>
   <si>
-    <t xml:space="preserve">Maximální krátkodobý výstupní proud (DC, 1s) </t>
+    <t xml:space="preserve">Maximum short-term output current (DC, 1s) </t>
   </si>
   <si>
     <t xml:space="preserve">15 A </t>
   </si>
   <si>
-    <t xml:space="preserve">Maximální výstupní výkon </t>
+    <t xml:space="preserve">Maximum output power </t>
   </si>
   <si>
     <t xml:space="preserve">3 200 W </t>
   </si>
   <si>
-    <t xml:space="preserve">Maximální brzdný výkon (interní rezistor) </t>
+    <t xml:space="preserve">Maximum braking power (internal resistor) </t>
   </si>
   <si>
     <t xml:space="preserve">100 W </t>
   </si>
   <si>
-    <t xml:space="preserve">Maximální brzdný výkon (externí rezistor) </t>
+    <t xml:space="preserve">Maximum braking power (external resistor) </t>
   </si>
   <si>
     <t xml:space="preserve">3 200 W</t>
   </si>
   <si>
-    <t xml:space="preserve">Ztráty při maximálním výstupním výkonu </t>
+    <t xml:space="preserve">Losses at maximum output power </t>
   </si>
   <si>
     <t xml:space="preserve">80 W </t>
   </si>
   <si>
-    <t xml:space="preserve">Jištění </t>
-  </si>
-  <si>
-    <t xml:space="preserve">16 A (char. Z, dvoupól)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VÝSTUPY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bezpotenciálový kontakt RDY</t>
+    <t xml:space="preserve">Overcurrent protection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 A (char. Z, dual)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OUTPUTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RDY digital output (contact)</t>
   </si>
   <si>
     <t xml:space="preserve">Max. 28 VDC / 700 mA</t>
   </si>
   <si>
-    <t xml:space="preserve">Bezpotenciálový kontakt ERR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1x zelená (Ready)  1x červená (Error)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KONEKTORY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Síťový napájecí konektor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DC bus konektor</t>
+    <t xml:space="preserve">ERR digital output (contact)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1x green (Ready)  1x red (Error)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONNECTORS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Network connector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DC bus connector</t>
   </si>
   <si>
     <t xml:space="preserve">1 x 8pin PHOENIX PC 5/ 8-STCL1-7,62</t>
   </si>
   <si>
-    <t xml:space="preserve">Konektor pro kontrolní výstupy</t>
+    <t xml:space="preserve">Digital outputs connector</t>
   </si>
   <si>
     <t xml:space="preserve">1 x 4pin WEIDMÜLLER BCZ 3.81/04/180 SN BK BX</t>
@@ -632,12 +638,24 @@
     <t xml:space="preserve">15 kW</t>
   </si>
   <si>
+    <t xml:space="preserve">Maximum braking power (internal resistor)</t>
+  </si>
+  <si>
     <t xml:space="preserve">400 W</t>
   </si>
   <si>
+    <t xml:space="preserve">Maximum braking power (external resistor)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Losses at maximum output power</t>
+  </si>
+  <si>
     <t xml:space="preserve">100 W</t>
   </si>
   <si>
+    <t xml:space="preserve">Fuse</t>
+  </si>
+  <si>
     <t xml:space="preserve">32 A</t>
   </si>
   <si>
@@ -656,7 +674,7 @@
     <t xml:space="preserve">1 x 7pin WAGO push-in</t>
   </si>
   <si>
-    <t xml:space="preserve">DI konektor</t>
+    <t xml:space="preserve">DI connector</t>
   </si>
   <si>
     <t xml:space="preserve">Připojení externího termistoru</t>
@@ -665,19 +683,19 @@
     <t xml:space="preserve">1x 2pin WEIDMÜLLER LSF (push-in)</t>
   </si>
   <si>
-    <t xml:space="preserve">Napájecí napětí</t>
+    <t xml:space="preserve">Supply voltage</t>
   </si>
   <si>
     <t xml:space="preserve">24 V DC (± 20 %)</t>
   </si>
   <si>
-    <t xml:space="preserve">Proudový odběr</t>
+    <t xml:space="preserve">Recommended PSU current</t>
   </si>
   <si>
     <t xml:space="preserve">min. 1 A</t>
   </si>
   <si>
-    <t xml:space="preserve">Napájení DO</t>
+    <t xml:space="preserve">DO supply</t>
   </si>
   <si>
     <t xml:space="preserve">Ethernet</t>
@@ -701,7 +719,7 @@
     <t xml:space="preserve">SD</t>
   </si>
   <si>
-    <t xml:space="preserve">microSD slot s detekcí vložené karty</t>
+    <t xml:space="preserve">microSD card slot with card detect</t>
   </si>
   <si>
     <t xml:space="preserve">HDMI</t>
@@ -710,13 +728,13 @@
     <t xml:space="preserve">standard A</t>
   </si>
   <si>
-    <t xml:space="preserve">stavová signalizační LED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Červená/zelená STS dioda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Napájení</t>
+    <t xml:space="preserve">status LED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">red/green STS diode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input power</t>
   </si>
   <si>
     <t xml:space="preserve">1 x 4pin WEIDMÜLLER BLF 2.50/04/180 SN BK BX</t>
@@ -731,40 +749,40 @@
     <t xml:space="preserve">2 x 10pin WEIDMÜLLER B2CF 3.50/10/180 SN OR BX</t>
   </si>
   <si>
-    <t xml:space="preserve">Červená/zelená dioda</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> č. vstupu </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> rozsah napětí log. 0 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> rozsah napětí log. 1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> nominální vstupní napětí </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> rozsah napájení DI/DO </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> spotřeba v log. 1 (17V) ±20% </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> spotřeba v log. 1 (24V) ±20% </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> vlastní spotřeba v log.1 (28V) ±20% </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Nominální vstupní odpor ±20%</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Přiřazeno k ose </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Max. vstupní frekvence - obdélník </t>
+    <t xml:space="preserve">red/green diode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input no.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">voltage range log. 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">voltage range log. 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nominal input voltage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">input supply range DI/DO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">consumption in log. 1 (17V) ±20%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">consumption in log. 1 (24V) ±20%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">consumption in log. 1 (28V) ±20%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nominal input resistance ±20%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assigned to axis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max. input frequency - rectangle</t>
   </si>
   <si>
     <t xml:space="preserve"> # </t>
@@ -794,100 +812,103 @@
     <t xml:space="preserve"> R&lt;sub&gt;in,Nom&lt;/sub&gt; </t>
   </si>
   <si>
+    <t xml:space="preserve">Ax. No.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> f&lt;sub&gt;max,Sq&lt;/sub&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> V</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> V </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> kΩ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-					 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kHz					 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0-10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 17-28V </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 17-28V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output no.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nominal output voltage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min. supply voltage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max. supply voltage 𐠒</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min. output voltage ±20%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max. output voltage ±20%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max. output current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assigned to axis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max. frequency - rectangle</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> VDD&lt;sub&gt;IO,min&lt;/sub&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> VDD&lt;sub&gt;IO,max&lt;/sub&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> V&lt;sub&gt;O,min&lt;/sub&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> V&lt;sub&gt;O,max&lt;/sub&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I&lt;sub&gt;O,max&lt;/sub&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Osa č. </t>
   </si>
   <si>
-    <t xml:space="preserve"> f&lt;sub&gt;max,Sq&lt;/sub&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> V</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> V </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> mA</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> kΩ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-					 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">kHz					 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0-10 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 17-28V </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 17-28V</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> nevyžaduje</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> č. výstupu </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> nominální výstupní napětí </t>
-  </si>
-  <si>
-    <t xml:space="preserve">min. napájecí napětí </t>
-  </si>
-  <si>
-    <t xml:space="preserve">max. napájecí napětí 𐠒 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">min.výstupní napětí ±20% </t>
-  </si>
-  <si>
-    <t xml:space="preserve">max. výstupní napětí ±20% </t>
-  </si>
-  <si>
-    <t xml:space="preserve">max. výstupní proud</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> přiřazeno k ose </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> max. frekvence - obdélník </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> VDD&lt;sub&gt;IO,min&lt;/sub&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> VDD&lt;sub&gt;IO,max&lt;/sub&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> V&lt;sub&gt;O,min&lt;/sub&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> V&lt;sub&gt;O,max&lt;/sub&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> I&lt;sub&gt;O,max&lt;/sub&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve"> f&lt;sub&gt;maxSq&lt;/sub&gt;</t>
   </si>
   <si>
     <t xml:space="preserve"> VDD&lt;sub&gt;IO&lt;/sub&gt; - 0,2</t>
   </si>
   <si>
-    <t xml:space="preserve"> rozsah napětí</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> nom. vstupní odpor ±10%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">časová konstanta ±10%</t>
+    <t xml:space="preserve">voltage range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nominal input resistance ±10%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time constant ±10%</t>
   </si>
   <si>
     <t xml:space="preserve"> V&lt;sub&gt;in&lt;/sub&gt; </t>
@@ -1156,12 +1177,12 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="38.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="48.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="52.92"/>
   </cols>
   <sheetData>
@@ -1376,7 +1397,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1398,7 +1419,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1406,7 +1427,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1414,7 +1435,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1422,7 +1443,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1438,7 +1459,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1534,7 +1555,7 @@
         <v>34</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1542,7 +1563,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1550,7 +1571,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1558,7 +1579,7 @@
         <v>40</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1566,20 +1587,20 @@
         <v>42</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1601,7 +1622,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1623,7 +1644,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1631,7 +1652,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1639,7 +1660,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1647,7 +1668,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1655,7 +1676,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1663,7 +1684,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1767,7 +1788,7 @@
         <v>34</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1775,7 +1796,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1783,7 +1804,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1791,7 +1812,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1799,7 +1820,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1821,7 +1842,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1843,7 +1864,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1851,7 +1872,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1859,7 +1880,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1867,7 +1888,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1875,7 +1896,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1987,7 +2008,7 @@
         <v>34</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1995,7 +2016,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2003,7 +2024,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2011,7 +2032,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2019,7 +2040,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2040,8 +2061,8 @@
   </sheetPr>
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2071,7 +2092,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2079,7 +2100,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2087,7 +2108,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2095,7 +2116,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2108,10 +2129,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2223,7 +2244,7 @@
         <v>34</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2231,7 +2252,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2239,7 +2260,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2247,7 +2268,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2255,7 +2276,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2264,16 +2285,16 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="B30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2295,7 +2316,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2325,7 +2346,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2333,7 +2354,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2341,7 +2362,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2362,10 +2383,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2477,7 +2498,7 @@
         <v>34</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2485,7 +2506,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2493,7 +2514,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2501,7 +2522,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2509,7 +2530,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2518,16 +2539,16 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="B30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2549,7 +2570,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2579,7 +2600,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2587,7 +2608,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2595,7 +2616,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2603,7 +2624,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2616,10 +2637,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2731,7 +2752,7 @@
         <v>34</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2739,7 +2760,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2747,7 +2768,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2755,7 +2776,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2763,7 +2784,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2772,16 +2793,16 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="B30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2803,7 +2824,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2833,7 +2854,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2841,7 +2862,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2849,7 +2870,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2857,7 +2878,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2865,15 +2886,15 @@
         <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2985,7 +3006,7 @@
         <v>34</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2993,7 +3014,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3001,7 +3022,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3009,7 +3030,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3017,7 +3038,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3026,16 +3047,16 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="B30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -3057,7 +3078,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3079,7 +3100,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3087,7 +3108,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3095,7 +3116,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3103,7 +3124,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3111,7 +3132,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3127,7 +3148,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3172,7 +3193,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>153</v>
+        <v>25</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>1</v>
@@ -3223,7 +3244,7 @@
         <v>34</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3231,7 +3252,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3247,7 +3268,7 @@
         <v>52</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3255,7 +3276,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3263,20 +3284,20 @@
         <v>42</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -3298,7 +3319,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3318,91 +3339,91 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C11" s="3"/>
     </row>
@@ -3417,7 +3438,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>1</v>
@@ -3425,18 +3446,18 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3452,12 +3473,12 @@
         <v>58</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>1</v>
@@ -3465,26 +3486,26 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -3506,7 +3527,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3526,16 +3547,16 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -3544,25 +3565,25 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>46</v>
@@ -3571,25 +3592,25 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>172</v>
+        <v>197</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="C8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>174</v>
+        <v>199</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>1</v>
@@ -3598,19 +3619,19 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>176</v>
+        <v>200</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="C10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>178</v>
+        <v>202</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="C11" s="3"/>
     </row>
@@ -3625,7 +3646,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>1</v>
@@ -3633,18 +3654,18 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3660,12 +3681,12 @@
         <v>58</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>1</v>
@@ -3676,12 +3697,12 @@
         <v>36</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>1</v>
@@ -3689,7 +3710,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>1</v>
@@ -3697,10 +3718,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -3722,7 +3743,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3950,7 +3971,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3973,21 +3994,21 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>46</v>
@@ -3996,16 +4017,16 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>46</v>
@@ -4014,7 +4035,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>56</v>
@@ -4023,25 +4044,25 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="C9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>1</v>
@@ -4050,19 +4071,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="C11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>178</v>
+        <v>202</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="C12" s="3"/>
     </row>
@@ -4077,7 +4098,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>1</v>
@@ -4085,18 +4106,18 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4112,12 +4133,12 @@
         <v>58</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>1</v>
@@ -4128,47 +4149,47 @@
         <v>36</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -4190,7 +4211,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4210,28 +4231,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -4249,19 +4270,19 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="C7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="C8" s="3"/>
     </row>
@@ -4276,28 +4297,28 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="C10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="C11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="C12" s="3"/>
     </row>
@@ -4315,16 +4336,16 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="C15" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>1</v>
@@ -4332,10 +4353,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4343,15 +4364,15 @@
         <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -4373,7 +4394,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4393,28 +4414,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -4459,10 +4480,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="C10" s="3"/>
     </row>
@@ -4480,10 +4501,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="C13" s="3"/>
     </row>
@@ -4492,7 +4513,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>1</v>
@@ -4501,7 +4522,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>37</v>
@@ -4512,7 +4533,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4520,7 +4541,7 @@
         <v>26</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4528,7 +4549,7 @@
         <v>40</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4536,7 +4557,7 @@
         <v>42</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -4558,7 +4579,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4578,28 +4599,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -4644,10 +4665,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="C10" s="3"/>
     </row>
@@ -4665,10 +4686,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="C13" s="3"/>
     </row>
@@ -4677,7 +4698,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>1</v>
@@ -4689,7 +4710,7 @@
         <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4697,7 +4718,7 @@
         <v>26</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -4716,10 +4737,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4737,107 +4758,107 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>239</v>
+        <v>244</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4845,16 +4866,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>2.05</v>
@@ -4880,16 +4901,16 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>2.05</v>
@@ -4915,16 +4936,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>2.05</v>
@@ -4950,16 +4971,16 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>2.05</v>
@@ -4985,16 +5006,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>2.05</v>
@@ -5020,16 +5041,16 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>2.05</v>
@@ -5055,16 +5076,16 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="F10" s="1" t="n">
         <v>1.25</v>
@@ -5090,16 +5111,16 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="F11" s="1" t="n">
         <v>1.25</v>
@@ -5119,6 +5140,18 @@
       <c r="K11" s="1" t="n">
         <v>50</v>
       </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0"/>
+      <c r="C19" s="0"/>
+      <c r="D19" s="0"/>
+      <c r="E19" s="0"/>
+      <c r="F19" s="0"/>
+      <c r="G19" s="0"/>
+      <c r="H19" s="0"/>
+      <c r="I19" s="0"/>
+      <c r="J19" s="0"/>
+      <c r="K19" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5136,10 +5169,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5156,117 +5189,117 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>263</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>266</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>267</v>
-      </c>
-      <c r="G1" s="0" t="s">
         <v>268</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>269</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>275</v>
+      </c>
       <c r="I1" s="0" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>243</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>271</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>272</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>273</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>274</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>275</v>
-      </c>
-      <c r="H2" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="I2" s="0" t="s">
-        <v>276</v>
+      <c r="C2" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>252</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>253</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>253</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>253</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>253</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>256</v>
-      </c>
-      <c r="I3" s="0" t="s">
         <v>257</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>277</v>
-      </c>
-      <c r="G4" s="0" t="n">
+      <c r="F4" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="G4" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="H4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" s="0" t="n">
+      <c r="H4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -5274,28 +5307,28 @@
       <c r="A5" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="F5" s="0" t="s">
-        <v>277</v>
-      </c>
-      <c r="G5" s="0" t="n">
+      <c r="F5" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="G5" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="I5" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -5303,28 +5336,28 @@
       <c r="A6" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>277</v>
-      </c>
-      <c r="G6" s="0" t="n">
+      <c r="F6" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="G6" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="H6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I6" s="0" t="n">
+      <c r="H6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -5332,28 +5365,28 @@
       <c r="A7" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="F7" s="0" t="s">
-        <v>277</v>
-      </c>
-      <c r="G7" s="0" t="n">
+      <c r="F7" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="G7" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="I7" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -5361,28 +5394,28 @@
       <c r="A8" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="F8" s="0" t="s">
-        <v>277</v>
-      </c>
-      <c r="G8" s="0" t="n">
+      <c r="F8" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="G8" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="H8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" s="0" t="n">
+      <c r="H8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -5390,63 +5423,40 @@
       <c r="A9" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="F9" s="0" t="s">
-        <v>277</v>
-      </c>
-      <c r="G9" s="0" t="n">
+      <c r="F9" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="G9" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="H9" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I9" s="0" t="n">
+      <c r="I9" s="1" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0"/>
-      <c r="B10" s="0"/>
-      <c r="C10" s="0"/>
-      <c r="D10" s="0"/>
-      <c r="E10" s="0"/>
-      <c r="F10" s="0"/>
-      <c r="G10" s="0"/>
-      <c r="H10" s="0"/>
-      <c r="I10" s="0"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0"/>
-      <c r="B11" s="0"/>
-      <c r="C11" s="0"/>
-      <c r="D11" s="0"/>
-      <c r="E11" s="0"/>
-      <c r="F11" s="0"/>
-      <c r="G11" s="0"/>
-      <c r="H11" s="0"/>
-      <c r="I11" s="0"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0"/>
-      <c r="B12" s="0"/>
-      <c r="C12" s="0"/>
-      <c r="D12" s="0"/>
-      <c r="E12" s="0"/>
-      <c r="F12" s="0"/>
-      <c r="G12" s="0"/>
-      <c r="H12" s="0"/>
-      <c r="I12" s="0"/>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0"/>
+      <c r="C19" s="0"/>
+      <c r="D19" s="0"/>
+      <c r="E19" s="0"/>
+      <c r="F19" s="0"/>
+      <c r="G19" s="0"/>
+      <c r="H19" s="0"/>
+      <c r="I19" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5464,10 +5474,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5480,44 +5490,44 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5525,7 +5535,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>11</v>
@@ -5539,7 +5549,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>11</v>
@@ -5547,6 +5557,11 @@
       <c r="D5" s="1" t="n">
         <v>22</v>
       </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0"/>
+      <c r="C13" s="0"/>
+      <c r="D13" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5567,7 +5582,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5787,7 +5802,7 @@
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6034,7 +6049,7 @@
   <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6286,12 +6301,12 @@
   <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="46.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
   </cols>
   <sheetData>
@@ -6505,7 +6520,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>94</v>
@@ -6538,12 +6553,12 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="38.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
   </cols>
   <sheetData>
@@ -6560,7 +6575,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6656,7 +6671,7 @@
         <v>26</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6679,8 +6694,8 @@
       <c r="A20" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>100</v>
+      <c r="B20" s="4" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6696,7 +6711,7 @@
         <v>34</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6704,7 +6719,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6728,7 +6743,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6736,12 +6751,12 @@
         <v>42</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>94</v>
@@ -6766,7 +6781,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6788,7 +6803,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6924,7 +6939,7 @@
         <v>34</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6932,7 +6947,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6969,7 +6984,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>94</v>
@@ -6994,7 +7009,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7016,7 +7031,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7048,7 +7063,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7152,7 +7167,7 @@
         <v>34</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7160,7 +7175,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7197,7 +7212,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
removed tab folder from each TGZ subfolder (redundant) finished translation of TGZ section (devices + modules) corrected errors in parametersEN
</commit_message>
<xml_diff>
--- a/docs/Manual/source/tab/parametersEN.xlsx
+++ b/docs/Manual/source/tab/parametersEN.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="TGZ-D-48-13_26" sheetId="1" state="visible" r:id="rId3"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="293">
   <si>
     <t xml:space="preserve">POWER SUPPLY</t>
   </si>
@@ -407,7 +407,7 @@
     <t xml:space="preserve">24 VDC ± 10 %, 600 mA*</t>
   </si>
   <si>
-    <t xml:space="preserve">0-320 VDC (pojistka 10 A)</t>
+    <t xml:space="preserve">0-320 VDC (fuse 10 A)</t>
   </si>
   <si>
     <t xml:space="preserve">2,6 kW</t>
@@ -417,6 +417,9 @@
   </si>
   <si>
     <t xml:space="preserve">2 x 10 A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED signaling (axis 1 and 2 separately)</t>
   </si>
   <si>
     <t xml:space="preserve">1 x 3pin PHOENIX  PC 5/ 3-STCL1-7,62  </t>
@@ -1622,7 +1625,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1769,7 +1772,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>31</v>
+        <v>124</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>32</v>
@@ -1788,7 +1791,7 @@
         <v>34</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1804,7 +1807,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1842,7 +1845,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1872,7 +1875,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1989,7 +1992,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>31</v>
+        <v>124</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>32</v>
@@ -2008,7 +2011,7 @@
         <v>34</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2024,7 +2027,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2061,7 +2064,7 @@
   </sheetPr>
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -2092,7 +2095,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2100,7 +2103,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2108,7 +2111,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2116,7 +2119,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2129,10 +2132,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2244,7 +2247,7 @@
         <v>34</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2260,7 +2263,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2285,7 +2288,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B30" s="3"/>
     </row>
@@ -2294,7 +2297,7 @@
         <v>117</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2346,7 +2349,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2354,7 +2357,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2362,7 +2365,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2383,10 +2386,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2498,7 +2501,7 @@
         <v>34</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2514,7 +2517,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2539,7 +2542,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B30" s="3"/>
     </row>
@@ -2548,7 +2551,7 @@
         <v>117</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2600,7 +2603,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2608,7 +2611,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2616,7 +2619,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2624,7 +2627,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2637,10 +2640,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2752,7 +2755,7 @@
         <v>34</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2768,7 +2771,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2793,7 +2796,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B30" s="3"/>
     </row>
@@ -2802,7 +2805,7 @@
         <v>117</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2854,7 +2857,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2862,7 +2865,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2870,7 +2873,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2878,7 +2881,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2886,15 +2889,15 @@
         <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3006,7 +3009,7 @@
         <v>34</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3022,7 +3025,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3047,7 +3050,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B30" s="3"/>
     </row>
@@ -3056,7 +3059,7 @@
         <v>117</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -3100,7 +3103,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3108,7 +3111,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3116,7 +3119,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3124,7 +3127,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3132,7 +3135,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3148,7 +3151,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3244,7 +3247,7 @@
         <v>34</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3252,7 +3255,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3268,7 +3271,7 @@
         <v>52</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3276,7 +3279,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3284,12 +3287,12 @@
         <v>42</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3297,7 +3300,7 @@
         <v>117</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -3339,91 +3342,91 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C11" s="3"/>
     </row>
@@ -3438,7 +3441,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>1</v>
@@ -3446,18 +3449,18 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3473,12 +3476,12 @@
         <v>58</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>1</v>
@@ -3486,26 +3489,26 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -3547,16 +3550,16 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -3565,25 +3568,25 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>46</v>
@@ -3592,25 +3595,25 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>1</v>
@@ -3619,19 +3622,19 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C11" s="3"/>
     </row>
@@ -3646,7 +3649,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>1</v>
@@ -3654,18 +3657,18 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3681,12 +3684,12 @@
         <v>58</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>1</v>
@@ -3697,12 +3700,12 @@
         <v>36</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>1</v>
@@ -3710,7 +3713,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>1</v>
@@ -3718,10 +3721,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -3994,21 +3997,21 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>46</v>
@@ -4017,16 +4020,16 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>46</v>
@@ -4035,7 +4038,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>56</v>
@@ -4044,25 +4047,25 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>1</v>
@@ -4071,19 +4074,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C12" s="3"/>
     </row>
@@ -4098,7 +4101,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>1</v>
@@ -4106,18 +4109,18 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4133,12 +4136,12 @@
         <v>58</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>1</v>
@@ -4149,47 +4152,47 @@
         <v>36</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -4231,28 +4234,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -4270,19 +4273,19 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C8" s="3"/>
     </row>
@@ -4297,28 +4300,28 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C12" s="3"/>
     </row>
@@ -4336,16 +4339,16 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C15" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>1</v>
@@ -4353,10 +4356,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4364,15 +4367,15 @@
         <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -4414,28 +4417,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -4480,10 +4483,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C10" s="3"/>
     </row>
@@ -4501,10 +4504,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C13" s="3"/>
     </row>
@@ -4513,7 +4516,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>1</v>
@@ -4522,7 +4525,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>37</v>
@@ -4533,7 +4536,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4578,8 +4581,8 @@
   </sheetPr>
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4599,28 +4602,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -4665,10 +4668,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C10" s="3"/>
     </row>
@@ -4686,10 +4689,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C13" s="3"/>
     </row>
@@ -4698,7 +4701,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>1</v>
@@ -4710,7 +4713,7 @@
         <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4737,7 +4740,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
@@ -4758,107 +4761,107 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="K1" s="0" t="s">
         <v>245</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4866,16 +4869,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>2.05</v>
@@ -4901,16 +4904,16 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>2.05</v>
@@ -4936,16 +4939,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>2.05</v>
@@ -4971,16 +4974,16 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>2.05</v>
@@ -5006,16 +5009,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>2.05</v>
@@ -5041,16 +5044,16 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>2.05</v>
@@ -5076,16 +5079,16 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="F10" s="1" t="n">
         <v>1.25</v>
@@ -5111,16 +5114,16 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="F11" s="1" t="n">
         <v>1.25</v>
@@ -5140,18 +5143,6 @@
       <c r="K11" s="1" t="n">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="0"/>
-      <c r="C19" s="0"/>
-      <c r="D19" s="0"/>
-      <c r="E19" s="0"/>
-      <c r="F19" s="0"/>
-      <c r="G19" s="0"/>
-      <c r="H19" s="0"/>
-      <c r="I19" s="0"/>
-      <c r="J19" s="0"/>
-      <c r="K19" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5169,7 +5160,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
@@ -5189,89 +5180,89 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="I1" s="0" t="s">
         <v>276</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5291,7 +5282,7 @@
         <v>0.5</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>300</v>
@@ -5320,7 +5311,7 @@
         <v>0.5</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>300</v>
@@ -5349,7 +5340,7 @@
         <v>0.5</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="G6" s="1" t="n">
         <v>300</v>
@@ -5378,7 +5369,7 @@
         <v>0.5</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="G7" s="1" t="n">
         <v>300</v>
@@ -5407,7 +5398,7 @@
         <v>0.5</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="G8" s="1" t="n">
         <v>300</v>
@@ -5436,7 +5427,7 @@
         <v>0.5</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="G9" s="1" t="n">
         <v>300</v>
@@ -5447,16 +5438,6 @@
       <c r="I9" s="1" t="n">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="0"/>
-      <c r="C19" s="0"/>
-      <c r="D19" s="0"/>
-      <c r="E19" s="0"/>
-      <c r="F19" s="0"/>
-      <c r="G19" s="0"/>
-      <c r="H19" s="0"/>
-      <c r="I19" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5474,7 +5455,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
@@ -5490,44 +5471,44 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D1" s="0" t="s">
         <v>287</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5535,7 +5516,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>11</v>
@@ -5549,7 +5530,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>11</v>
@@ -5557,11 +5538,6 @@
       <c r="D5" s="1" t="n">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0"/>
-      <c r="C13" s="0"/>
-      <c r="D13" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>